<commit_message>
update exel data des
</commit_message>
<xml_diff>
--- a/DataQC.xlsx
+++ b/DataQC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\DATA PRODUCTION\Streamlit Data Barang\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\DATA PRODUCTION\Streamlit Data Barang\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -430,7 +430,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G15:H16"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,13 +613,13 @@
         <v>14</v>
       </c>
       <c r="B13" s="6">
-        <v>2328</v>
+        <v>2419</v>
       </c>
       <c r="C13" s="6">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="D13" s="3">
-        <v>434</v>
+        <v>455</v>
       </c>
     </row>
   </sheetData>

</xml_diff>